<commit_message>
Uitbreiding met Gronau en 2022
</commit_message>
<xml_diff>
--- a/Stationscodes.xlsx
+++ b/Stationscodes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Mobiliteit-projecten\OV_Oost_reizigers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9CFF29-C120-4FBE-9518-AD8A0EEA7F7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F42C131-B685-4503-A372-7231DCA7C9C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13485" yWindow="0" windowWidth="18000" windowHeight="9240" xr2:uid="{0CE0F5B6-8556-47E6-9FDF-B5EC4AD1392A}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11265" xr2:uid="{0CE0F5B6-8556-47E6-9FDF-B5EC4AD1392A}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
   <si>
     <t>HNR</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>45240001</t>
+  </si>
+  <si>
+    <t>Gronau</t>
   </si>
 </sst>
 </file>
@@ -542,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6F9838-ED03-4852-9CD1-56A337459079}">
-  <dimension ref="A1:G55"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56:B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -1058,6 +1061,14 @@
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
     </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>40</v>
+      </c>
+      <c r="B56">
+        <v>398</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D40:G55">
     <sortCondition ref="D40:D55"/>

</xml_diff>